<commit_message>
Implement more function and now we can open xlsx file and read sheet names
</commit_message>
<xml_diff>
--- a/tests/documents/testLoadXlsx.xlsx
+++ b/tests/documents/testLoadXlsx.xlsx
@@ -2,15 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -41,6 +47,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,8 +107,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,20 +141,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -156,4 +167,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.3418367346939"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>